<commit_message>
length of longest substring
</commit_message>
<xml_diff>
--- a/Data Structure/Sliding Window/Sliding Window.xlsx
+++ b/Data Structure/Sliding Window/Sliding Window.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Documents/Study Material/DS/DataStructure-And-Algorithm/Data Structure/Sliding Window/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828860FA-6F14-6945-B6BB-FC0602E72C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CD3446-2050-3A48-8B15-2CE5B12113C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4E42177B-4881-CA45-8674-08098C02AC7A}"/>
   </bookViews>
@@ -716,7 +716,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:C4"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
438. Find All Anagrams in a String
</commit_message>
<xml_diff>
--- a/Data Structure/Sliding Window/Sliding Window.xlsx
+++ b/Data Structure/Sliding Window/Sliding Window.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Documents/Study Material/DS/DataStructure-And-Algorithm/Data Structure/Sliding Window/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F91E35-8431-6E46-A942-FC4A27B6BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104C4639-9318-B349-8681-11FBBED4E051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4E42177B-4881-CA45-8674-08098C02AC7A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Number</t>
   </si>
@@ -195,54 +195,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Come Up with a Brute Force Approach
-2. Always check for base case.
-3. Mostly </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="4"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>dictionary</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> is used.
-4. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Dictonary and Set</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> are used for unique values.</t>
-    </r>
-  </si>
-  <si>
     <t>424. Longest Repeating Character Replacement.</t>
   </si>
   <si>
@@ -310,6 +262,123 @@
         <family val="1"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>438. Find All Anagrams in a String</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Come Up with a Brute Force Approach
+2. Always check for base case.
+3. Mostly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="4"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>dictionary</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> is used.
+4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Dictonary, Collections and Set</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> are used for unique values.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sliding Window
+Dictionary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Brute Force</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:
+Create a Collection Dictionary for both the array and check if they are the same.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2 pointer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Use 2 pointer left and right.
+As we move front add right to dict and remove left from dict. 
+Then compare the 2 dictionary.</t>
     </r>
   </si>
 </sst>
@@ -785,8 +854,8 @@
   <dimension ref="A1:C302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,7 +884,7 @@
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -902,16 +971,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="217" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>

</xml_diff>